<commit_message>
Make 2 test cases fail, add integration with cypress cloud for runs
</commit_message>
<xml_diff>
--- a/Cypress notes.xlsx
+++ b/Cypress notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\cypressAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AFFA17-FD53-4B73-B2D6-D465C41C5F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510EDD2-A0C8-4E6C-9575-608F55ECCE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B0DC8F9-F96A-4257-ABFF-25728A9A412A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>CSS selectors</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Generate reports</t>
+  </si>
+  <si>
+    <t>Command line for cypress</t>
+  </si>
+  <si>
+    <t>npx cypress run --spec cypress/integration/examples/test9.js --headed --record --key 06499df6-3ffe-4a1d-872f-f3aa072ec3b4</t>
+  </si>
+  <si>
+    <t>Run for cypress cloud and a specific test case in the spec and headed mode</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D6870B-BCCC-4953-9EDE-235F6CF02829}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,39 +590,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>